<commit_message>
ML_PL std reduced 60%
</commit_message>
<xml_diff>
--- a/ML_PL_new/actual_tx.xlsx
+++ b/ML_PL_new/actual_tx.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -437,7 +437,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -495,7 +495,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
@@ -800,13 +800,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="C62" sqref="A37:C62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
     <col min="4" max="9" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2500,7 +2501,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>45780.75</v>
       </c>

</xml_diff>